<commit_message>
Update Judi's supersite spreadsheet and save all files
</commit_message>
<xml_diff>
--- a/data/supersite_venues_all_years.xlsx
+++ b/data/supersite_venues_all_years.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/blueT7/bcdp/data/supersiteDB/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666DA041-459E-7943-B58C-49C7F2AEA175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C2150D-1859-E84E-A290-3E8E9E82F931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22360" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="500" windowWidth="29380" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="venues_all_known" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="188">
   <si>
     <t>Venue</t>
   </si>
@@ -579,6 +579,24 @@
   </si>
   <si>
     <t>geometry-invalid</t>
+  </si>
+  <si>
+    <t>700 20th St, Boulder, CO 80302</t>
+  </si>
+  <si>
+    <t>http://nvh.bvsd.org/</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
+  </si>
+  <si>
+    <t>New Vista High School</t>
+  </si>
+  <si>
+    <t>POINT (-105.2665043792843 40.00119784626813)</t>
+  </si>
+  <si>
+    <t>New Vista</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB5BB1E-7EF7-EA4C-80A4-9E907A862B21}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1068,11 +1086,11 @@
         <v>124</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D29" si="0">HYPERLINK(K2)</f>
+        <f t="shared" ref="D2:D30" si="0">HYPERLINK(K2)</f>
         <v>http://www.allensparkfire.com/</v>
       </c>
       <c r="E2" s="5" t="str">
-        <f t="shared" ref="E2:E30" si="1">HYPERLINK(J2)</f>
+        <f t="shared" ref="E2:E31" si="1">HYPERLINK(J2)</f>
         <v>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1864,247 +1882,277 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>187</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>https://nhs.svvsd.org/</v>
-      </c>
-      <c r="E24" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</v>
+        <v>130</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="H24" s="1">
-        <v>40.103695062172719</v>
+        <v>40.001197846268099</v>
       </c>
       <c r="I24" s="1">
-        <v>-105.1442414652976</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>-105.266504379284</v>
+      </c>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D25" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>http://schs.svvsd.org/</v>
+        <v>https://nhs.svvsd.org/</v>
       </c>
       <c r="E25" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/6j7ZvjGuNgq38Uv1A</v>
+        <v>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H25" s="1">
-        <v>40.151371607549947</v>
+        <v>40.103695062172719</v>
       </c>
       <c r="I25" s="1">
-        <v>-105.16656999308471</v>
+        <v>-105.1442414652976</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>http://shm.bvsd.org/</v>
+        <v>http://schs.svvsd.org/</v>
       </c>
       <c r="E26" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</v>
+        <v>https://maps.app.goo.gl/6j7ZvjGuNgq38Uv1A</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H26" s="1">
-        <v>39.974133893699872</v>
+        <v>40.151371607549947</v>
       </c>
       <c r="I26" s="1">
-        <v>-105.2452260530946</v>
+        <v>-105.16656999308471</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D27" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>http://sms.svvsd.org/</v>
+        <v>http://shm.bvsd.org/</v>
       </c>
       <c r="E27" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/2iVHM51MYZg9XEZo9</v>
+        <v>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H27" s="1">
-        <v>40.144580730699623</v>
+        <v>39.974133893699872</v>
       </c>
       <c r="I27" s="1">
-        <v>-105.11990671854279</v>
+        <v>-105.2452260530946</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D28" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>http://tpk8.svvsd.org/</v>
+        <v>http://sms.svvsd.org/</v>
       </c>
       <c r="E28" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/Dqyuok7JMiowX96x5</v>
+        <v>https://maps.app.goo.gl/2iVHM51MYZg9XEZo9</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H28" s="1">
-        <v>40.180911331524733</v>
+        <v>40.144580730699623</v>
       </c>
       <c r="I28" s="1">
-        <v>-105.0857347392096</v>
+        <v>-105.11990671854279</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>https://trms.svvsd.org/</v>
+        <v>http://tpk8.svvsd.org/</v>
       </c>
       <c r="E29" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</v>
+        <v>https://maps.app.goo.gl/Dqyuok7JMiowX96x5</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H29" s="1">
-        <v>40.176931177836657</v>
+        <v>40.180911331524733</v>
       </c>
       <c r="I29" s="1">
-        <v>-105.0576162268638</v>
+        <v>-105.0857347392096</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://trms.svvsd.org/</v>
+      </c>
+      <c r="E30" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="1">
+        <v>40.176931177836657</v>
+      </c>
+      <c r="I30" s="1">
+        <v>-105.0576162268638</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="7" t="str">
+      <c r="E31" s="7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H31" s="1">
         <v>40.073398440992797</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I31" s="1">
         <v>-105.506518983446</v>
       </c>
-      <c r="J30" s="6"/>
+      <c r="J31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>